<commit_message>
Pad zero for development convenience
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/BiDiagDecompTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/BiDiagDecompTest.xlsx
@@ -71,7 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,8 +86,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +111,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -131,20 +143,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:I12"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3985,7 +4000,7 @@
         <v>8.8817841970012523E-16</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" ref="A65:A73" si="76">AG52</f>
         <v>7.310494211901453E-16</v>
@@ -3999,7 +4014,7 @@
         <v>0.38196055250832472</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="76"/>
         <v>-1.0094684939496983E-15</v>
@@ -4013,7 +4028,7 @@
         <v>-30.651378914612064</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="76"/>
         <v>-1.8385961586756272E-17</v>
@@ -4027,7 +4042,7 @@
         <v>-5.5511151231257827E-16</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="76"/>
         <v>3.1256835270909162E-18</v>
@@ -4041,7 +4056,7 @@
         <v>3.5527136788005009E-15</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="76"/>
         <v>1.4024283862467174E-15</v>
@@ -4055,7 +4070,7 @@
         <v>4.4408920985006262E-15</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="76"/>
         <v>-4.5251892099652144E-16</v>
@@ -4069,7 +4084,7 @@
         <v>8.8817841970012523E-16</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="76"/>
         <v>2.9163031188788019E-16</v>
@@ -4083,7 +4098,7 @@
         <v>-2.7755575615628914E-17</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="76"/>
         <v>-2.9686478181005755E-16</v>
@@ -4097,7 +4112,7 @@
         <v>2.2204460492503131E-15</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="76"/>
         <v>5.099309236458049E-17</v>
@@ -4111,20 +4126,20 @@
         <v>-3.5527136788005009E-15</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1</v>
       </c>
       <c r="B76">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f>-F3</f>
         <v>-35.202840794458623</v>
@@ -4144,6 +4159,9 @@
       <c r="E77" s="1">
         <f>-F51</f>
         <v>-30.651378914612071</v>
+      </c>
+      <c r="F77" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4155,8 +4173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:K5"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5590,7 +5608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="F9" sqref="F9:J13"/>
     </sheetView>
   </sheetViews>
@@ -7485,7 +7503,7 @@
   <dimension ref="A1:Z66"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8066,7 +8084,7 @@
         <v>0.3669204023076606</v>
       </c>
       <c r="V11">
-        <f t="shared" ref="V11:V13" si="11">-2*Q11</f>
+        <f t="shared" ref="V11:V12" si="11">-2*Q11</f>
         <v>0.64249573043291219</v>
       </c>
     </row>
@@ -8118,7 +8136,7 @@
         <v>0</v>
       </c>
       <c r="T12">
-        <f t="shared" ref="T11:T13" si="14">-2*O12</f>
+        <f t="shared" ref="T12:T13" si="14">-2*O12</f>
         <v>0.3669204023076606</v>
       </c>
       <c r="U12">
@@ -8401,7 +8419,7 @@
         <v>-5.4104286416236125</v>
       </c>
       <c r="J19">
-        <f t="shared" ref="J18:J22" si="21">H19</f>
+        <f t="shared" ref="J19:J22" si="21">H19</f>
         <v>-5.4104286416236125</v>
       </c>
       <c r="L19">
@@ -8846,7 +8864,7 @@
         <v>-1.2789201619438555</v>
       </c>
       <c r="J27">
-        <f t="shared" ref="J26:J27" si="32">H27</f>
+        <f t="shared" ref="J27" si="32">H27</f>
         <v>-1.2789201619438555</v>
       </c>
       <c r="L27">
@@ -9166,7 +9184,7 @@
         <v>-7.4730865218796625</v>
       </c>
       <c r="J34">
-        <f t="shared" ref="J33:J36" si="41">H34</f>
+        <f t="shared" ref="J34:J36" si="41">H34</f>
         <v>-7.4730865218796625</v>
       </c>
       <c r="L34">
@@ -9769,7 +9787,7 @@
         <v>2.0488517690421952</v>
       </c>
       <c r="J49">
-        <f t="shared" ref="J48:J50" si="57">H49</f>
+        <f t="shared" ref="J49:J50" si="57">H49</f>
         <v>2.0488517690421952</v>
       </c>
       <c r="L49">
@@ -10077,15 +10095,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1</v>
       </c>
       <c r="B65">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f>A59</f>
         <v>12.401225109178808</v>
@@ -10113,6 +10131,9 @@
       <c r="G66" s="1">
         <f>D62</f>
         <v>9.3999696866547335</v>
+      </c>
+      <c r="H66" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -10124,8 +10145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:W7"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10529,7 +10550,7 @@
         <v>31.58701836407355</v>
       </c>
       <c r="K9">
-        <f t="shared" ref="K9:K13" si="8">I9/J$3</f>
+        <f t="shared" ref="K9" si="8">I9/J$3</f>
         <v>0</v>
       </c>
       <c r="M9">
@@ -11010,7 +11031,7 @@
         <v>6.5533355571608283</v>
       </c>
       <c r="I19">
-        <f t="shared" ref="I18:I21" si="24">G19</f>
+        <f t="shared" ref="I19:I21" si="24">G19</f>
         <v>6.5533355571608283</v>
       </c>
       <c r="K19">
@@ -11213,7 +11234,7 @@
         <v>14.787727780918033</v>
       </c>
       <c r="K23">
-        <f t="shared" ref="K23:K27" si="28">I23/J$3</f>
+        <f t="shared" ref="K23" si="28">I23/J$3</f>
         <v>0</v>
       </c>
       <c r="M23">
@@ -11400,7 +11421,7 @@
         <v>-7.8374211781037273</v>
       </c>
       <c r="I26">
-        <f t="shared" ref="I25:I27" si="35">G26</f>
+        <f t="shared" ref="I26:I27" si="35">G26</f>
         <v>-7.8374211781037273</v>
       </c>
       <c r="K26">
@@ -11757,7 +11778,7 @@
         <v>6.7675687215963629</v>
       </c>
       <c r="I34">
-        <f t="shared" ref="I33:I35" si="45">G34</f>
+        <f t="shared" ref="I34:I35" si="45">G34</f>
         <v>6.7675687215963629</v>
       </c>
       <c r="K34">
@@ -11896,7 +11917,7 @@
         <v>18.057844010965528</v>
       </c>
       <c r="K37">
-        <f t="shared" ref="K37:K41" si="48">I37/J$3</f>
+        <f t="shared" ref="K37" si="48">I37/J$3</f>
         <v>0</v>
       </c>
       <c r="M37">
@@ -12146,7 +12167,7 @@
         <v>-6.3052818377802655</v>
       </c>
       <c r="I41">
-        <f t="shared" ref="I40:I41" si="56">G41</f>
+        <f t="shared" ref="I41" si="56">G41</f>
         <v>-6.3052818377802655</v>
       </c>
       <c r="K41">
@@ -12503,7 +12524,7 @@
         <v>3.1077738016288157</v>
       </c>
       <c r="I49">
-        <f t="shared" ref="I48:I49" si="65">G49</f>
+        <f t="shared" ref="I49" si="65">G49</f>
         <v>3.1077738016288157</v>
       </c>
       <c r="K49">
@@ -12642,7 +12663,7 @@
         <v>1</v>
       </c>
       <c r="B58">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.25">
@@ -12681,6 +12702,9 @@
       <c r="I59" s="1">
         <f>E55</f>
         <v>1.8929822833086383</v>
+      </c>
+      <c r="J59" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -12692,8 +12716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63:I64"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12766,7 +12790,7 @@
         <v>20.882925302146504</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K7" si="0">I3/J$3</f>
+        <f t="shared" ref="K3" si="0">I3/J$3</f>
         <v>-0.78959441606214575</v>
       </c>
       <c r="M3">
@@ -13215,7 +13239,7 @@
         <v>0.79005229194906545</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I10:I13" si="7">G11</f>
+        <f t="shared" ref="I11:I13" si="7">G11</f>
         <v>0.79005229194906545</v>
       </c>
       <c r="K11">
@@ -13450,7 +13474,7 @@
         <v>17.089514564369903</v>
       </c>
       <c r="K17">
-        <f t="shared" ref="K17:K21" si="8">I17/J$3</f>
+        <f t="shared" ref="K17" si="8">I17/J$3</f>
         <v>0</v>
       </c>
       <c r="M17">
@@ -13474,15 +13498,15 @@
         <v>1</v>
       </c>
       <c r="T17">
-        <f t="shared" ref="T17:T20" si="9">-2*N17</f>
+        <f t="shared" ref="T17" si="9">-2*N17</f>
         <v>0</v>
       </c>
       <c r="U17">
-        <f t="shared" ref="U17:U20" si="10">-2*O17</f>
+        <f t="shared" ref="U17:U18" si="10">-2*O17</f>
         <v>0</v>
       </c>
       <c r="V17">
-        <f t="shared" ref="V17:V20" si="11">-2*P17</f>
+        <f t="shared" ref="V17:V19" si="11">-2*P17</f>
         <v>0</v>
       </c>
       <c r="W17">
@@ -13799,19 +13823,19 @@
         <v>1</v>
       </c>
       <c r="T23">
-        <f t="shared" ref="T23:T27" si="18">-2*N23</f>
+        <f t="shared" ref="T23" si="18">-2*N23</f>
         <v>0</v>
       </c>
       <c r="U23">
-        <f t="shared" ref="U23:U27" si="19">-2*O23</f>
+        <f t="shared" ref="U23:U24" si="19">-2*O23</f>
         <v>0</v>
       </c>
       <c r="V23">
-        <f t="shared" ref="V23:V27" si="20">-2*P23</f>
+        <f t="shared" ref="V23:V25" si="20">-2*P23</f>
         <v>0</v>
       </c>
       <c r="W23">
-        <f t="shared" ref="W23:W27" si="21">-2*Q23</f>
+        <f t="shared" ref="W23:W26" si="21">-2*Q23</f>
         <v>0</v>
       </c>
     </row>
@@ -13963,7 +13987,7 @@
         <v>12.448813318744556</v>
       </c>
       <c r="I26">
-        <f t="shared" ref="I25:I27" si="25">G26</f>
+        <f t="shared" ref="I26:I27" si="25">G26</f>
         <v>12.448813318744556</v>
       </c>
       <c r="K26">
@@ -14134,7 +14158,7 @@
         <v>13.740550043919827</v>
       </c>
       <c r="K31">
-        <f t="shared" ref="K31:K35" si="28">I31/J$3</f>
+        <f t="shared" ref="K31" si="28">I31/J$3</f>
         <v>0</v>
       </c>
       <c r="M31">
@@ -14158,15 +14182,15 @@
         <v>1</v>
       </c>
       <c r="T31">
-        <f t="shared" ref="T31:T34" si="29">-2*N31</f>
+        <f t="shared" ref="T31" si="29">-2*N31</f>
         <v>0</v>
       </c>
       <c r="U31">
-        <f t="shared" ref="U31:U34" si="30">-2*O31</f>
+        <f t="shared" ref="U31:U32" si="30">-2*O31</f>
         <v>0</v>
       </c>
       <c r="V31">
-        <f t="shared" ref="V31:V34" si="31">-2*P31</f>
+        <f t="shared" ref="V31:V33" si="31">-2*P31</f>
         <v>0</v>
       </c>
       <c r="W31">
@@ -14321,7 +14345,7 @@
         <v>3.4965344039406823</v>
       </c>
       <c r="I34">
-        <f t="shared" ref="I33:I35" si="35">G34</f>
+        <f t="shared" ref="I34:I35" si="35">G34</f>
         <v>3.4965344039406823</v>
       </c>
       <c r="K34">
@@ -14483,19 +14507,19 @@
         <v>1</v>
       </c>
       <c r="T37">
-        <f t="shared" ref="T37:T41" si="38">-2*N37</f>
+        <f t="shared" ref="T37" si="38">-2*N37</f>
         <v>0</v>
       </c>
       <c r="U37">
-        <f t="shared" ref="U37:U41" si="39">-2*O37</f>
+        <f t="shared" ref="U37:U38" si="39">-2*O37</f>
         <v>0</v>
       </c>
       <c r="V37">
-        <f t="shared" ref="V37:V41" si="40">-2*P37</f>
+        <f t="shared" ref="V37:V39" si="40">-2*P37</f>
         <v>0</v>
       </c>
       <c r="W37">
-        <f t="shared" ref="W37:W41" si="41">-2*Q37</f>
+        <f t="shared" ref="W37:W40" si="41">-2*Q37</f>
         <v>0</v>
       </c>
     </row>
@@ -14710,7 +14734,7 @@
         <v>-1.0276228042268194</v>
       </c>
       <c r="I41">
-        <f t="shared" ref="I40:I41" si="45">G41</f>
+        <f t="shared" ref="I41" si="45">G41</f>
         <v>-1.0276228042268194</v>
       </c>
       <c r="K41">
@@ -14817,7 +14841,7 @@
         <v>22.308115056771705</v>
       </c>
       <c r="K45">
-        <f t="shared" ref="K45:K49" si="47">I45/J$3</f>
+        <f t="shared" ref="K45" si="47">I45/J$3</f>
         <v>0</v>
       </c>
       <c r="M45">
@@ -14841,15 +14865,15 @@
         <v>1</v>
       </c>
       <c r="T45">
-        <f t="shared" ref="T45:T48" si="48">-2*N45</f>
+        <f t="shared" ref="T45" si="48">-2*N45</f>
         <v>0</v>
       </c>
       <c r="U45">
-        <f t="shared" ref="U45:U48" si="49">-2*O45</f>
+        <f t="shared" ref="U45:U46" si="49">-2*O45</f>
         <v>0</v>
       </c>
       <c r="V45">
-        <f t="shared" ref="V45:V48" si="50">-2*P45</f>
+        <f t="shared" ref="V45:V47" si="50">-2*P45</f>
         <v>0</v>
       </c>
       <c r="W45">
@@ -15067,7 +15091,7 @@
         <v>10.485059200425423</v>
       </c>
       <c r="I49">
-        <f t="shared" ref="I48:I49" si="55">G49</f>
+        <f t="shared" ref="I49" si="55">G49</f>
         <v>10.485059200425423</v>
       </c>
       <c r="K49">
@@ -15319,20 +15343,20 @@
         <v>3.9430916136518879</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1</v>
       </c>
       <c r="B66">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f>A59</f>
         <v>13.22383041048691</v>
@@ -15368,6 +15392,9 @@
       <c r="I67" s="1">
         <f>E63</f>
         <v>3.9430916136518879</v>
+      </c>
+      <c r="J67" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -15388,1051 +15415,1051 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*20-7</f>
-        <v>-4.8004842473042295</v>
+        <v>12.041620907257133</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:J16" ca="1" si="0">RAND()*20-7</f>
-        <v>5.9685244968874969</v>
+        <v>-4.5802676133425244</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>7.6174035749420383</v>
+        <v>9.3088409042958382</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>5.9486938677202836</v>
+        <v>-4.6930478936307818</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>12.204417933418409</v>
+        <v>-5.3750324880874221</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>11.958052031947496</v>
+        <v>10.671306160962942</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.98049034129849044</v>
+        <v>5.0068654950857159</v>
       </c>
       <c r="H1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46728686992627466</v>
+        <v>11.31171318170583</v>
       </c>
       <c r="I1">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.6167595285917349</v>
+        <v>1.1899712577687911</v>
       </c>
       <c r="J1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1182617305667275</v>
+        <v>11.982372606055606</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:J25" ca="1" si="1">RAND()*20-7</f>
-        <v>4.566833520224959</v>
+        <v>11.040020259804567</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>10.963218343159802</v>
+        <v>8.650627484989176</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>12.892323793337479</v>
+        <v>-1.7058279279778219</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2106898389246705</v>
+        <v>1.0627199231574824</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2220837608751793</v>
+        <v>10.75817091785807</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2491708670857857</v>
+        <v>2.2669898275966371</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>12.668171396108839</v>
+        <v>-4.1117722051896237</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.7026797583625362</v>
+        <v>1.1052114381397722</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7353945671329978</v>
+        <v>-0.30174037270263021</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8695538815467092</v>
+        <v>5.5855014627110684</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>6.2376415217118151</v>
+        <v>-0.82951939429402799</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4727656621652638</v>
+        <v>6.2017333660497442E-2</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.7650166641206502</v>
+        <v>-3.7766554027024783</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>10.540369995134412</v>
+        <v>4.2559003668537994</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8569585058250198</v>
+        <v>6.3024008114219168</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5915093475713213</v>
+        <v>12.295908047108579</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.8715327861586442</v>
+        <v>9.0198049862516783E-2</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.6672537476002933</v>
+        <v>-4.4421318893783939</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.7805919653796209</v>
+        <v>0.4332526004210786</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5990315214660136</v>
+        <v>-2.56263882823073</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.71160223992659155</v>
+        <v>12.702803793125113</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7242490432324438</v>
+        <v>12.186786362075701</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.3487105623128781</v>
+        <v>-3.3103405842571791</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>11.939712309763401</v>
+        <v>1.6783787927134775</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>5.4958276788688813</v>
+        <v>2.3301887354713813</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>10.409070345958988</v>
+        <v>-3.6150199462329318</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>12.017962278122056</v>
+        <v>6.7557936953498157</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>7.6673343498455271</v>
+        <v>7.4454147112899722</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>7.1132071674131865</v>
+        <v>-2.134031697531154</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.780835157844832</v>
+        <v>11.898068851429066</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.3050137597373528</v>
+        <v>-4.2737377261350877</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.4318360083067381</v>
+        <v>3.6898886414609926</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.0734876284432966</v>
+        <v>8.3548418855072288</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5577853143144598</v>
+        <v>-5.8025507530212632</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.9336445262055095</v>
+        <v>-3.7222318668603553</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5566804624287762</v>
+        <v>-1.5873423305145433</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9138193390161575</v>
+        <v>-4.3159895327820053E-3</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5012144636068019</v>
+        <v>4.0348438693420157</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>11.287131038737204</v>
+        <v>-6.80268828152004</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.6984847916649386</v>
+        <v>2.189298359896279</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>2.982285803252859</v>
+        <v>12.977699517501598</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.5908865656604965</v>
+        <v>4.1611918759469742</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>9.0205927884849899</v>
+        <v>-2.7413077471102447</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>12.120368452540507</v>
+        <v>-1.2366711097496683</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.5792239648991329</v>
+        <v>6.9153586148973858</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>8.7829169247197889</v>
+        <v>8.7894594954153114</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4876852424563189</v>
+        <v>-4.1436967593069056</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.2508042549564289</v>
+        <v>2.8162087810901095</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70071407495386051</v>
+        <v>10.816626076116126</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>10.293543702272896</v>
+        <v>9.4373103146605182</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.6090131617812098</v>
+        <v>4.7252795755223858</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.6061912127620492</v>
+        <v>11.819411554080578</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>10.160309103180509</v>
+        <v>9.5421868592796457</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>11.729453865114834</v>
+        <v>8.7068351092706138</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0785453317613332</v>
+        <v>4.1229266747658713</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>8.7060432008619486</v>
+        <v>9.9123475772176164</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>1.165757034106333</v>
+        <v>5.7833414032390351</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6838935818118248</v>
+        <v>7.8882287307315568</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.39326059009718506</v>
+        <v>5.6304564941224751</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>10.475908485784903</v>
+        <v>-3.0652368150552172</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.7414318068174115</v>
+        <v>-0.16510134525659126</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>10.011643333889996</v>
+        <v>-1.1698609455114859</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14353450097997289</v>
+        <v>-0.55286468444132808</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0710167079571455</v>
+        <v>12.587830323206255</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.0692373750980799</v>
+        <v>0.4333108635557128</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7722077058364594</v>
+        <v>9.591726815871418</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.4334453178867381</v>
+        <v>-3.7198612288885173</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.9530453175818012</v>
+        <v>6.5133560404554736</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9014941046352103</v>
+        <v>9.407777887627077</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>10.941615558270488</v>
+        <v>11.81449860195746</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.8029681006946099</v>
+        <v>11.658673447065215</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.1426579163531958</v>
+        <v>-6.7895845498578771</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.7853005472740868</v>
+        <v>-1.2917591983076147</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.0141731965156051</v>
+        <v>6.3762746644241588</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.3081568856135455</v>
+        <v>3.7399402716869794</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.3091931478723762</v>
+        <v>-1.2914455972573933</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.511386497338485</v>
+        <v>-3.7087814931833689</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9737083874424339</v>
+        <v>9.8231965596670676</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7159261301568947</v>
+        <v>1.5394391625247472</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.7021636776042737</v>
+        <v>3.4186912033654764</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.2762102856546309</v>
+        <v>-4.2363366003471956</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.5434573432977654</v>
+        <v>11.167014452695437</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.0155757053637604</v>
+        <v>11.335236052215677</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>10.041238142460831</v>
+        <v>9.468548460740724</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.9403700799021206</v>
+        <v>1.2731258442186739</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.5592523585452751</v>
+        <v>2.0590523907088745</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.3291801747091014</v>
+        <v>-5.0659589986443709</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0884044833245667</v>
+        <v>-2.0459255803909748</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.082586874351442</v>
+        <v>2.9440622972496904</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>9.0362603326214597</v>
+        <v>12.401851484455982</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>10.478227076169027</v>
+        <v>8.6906785032984999</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>8.3412564694221984</v>
+        <v>-1.3507642644073963</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.54779155131578872</v>
+        <v>-5.6558523203923121</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>11.079286547124383</v>
+        <v>4.4522642723228341</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.90968326677458577</v>
+        <v>6.0640116177586059</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4823005850611555</v>
+        <v>4.5547108789325499</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>8.7302547772061772</v>
+        <v>9.4990791901873166</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54058484589919864</v>
+        <v>-4.3416867617683153E-2</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.8879464269537554</v>
+        <v>0.11098712149333068</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>11.585356733515219</v>
+        <v>11.626530142484462</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>11.958152299809527</v>
+        <v>6.8579620280517339</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.77162475322005619</v>
+        <v>5.1298604161687038</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.8875265069444591</v>
+        <v>-2.1021371692975315</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.14544344077392779</v>
+        <v>2.9935676514544944</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2046607366592283</v>
+        <v>2.2743617182991009</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>8.9631348754989855</v>
+        <v>4.5837313671474558</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.3129842739522832</v>
+        <v>4.6936179671346459</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>12.079514569817206</v>
+        <v>4.7352442388976446</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9667902895653997</v>
+        <v>11.321012189351379</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>10.864689466611949</v>
+        <v>-1.2548770238295592</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3025248908518048</v>
+        <v>-3.9701736316058049</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.16358538906785114</v>
+        <v>11.666111087384781</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1852597504643292</v>
+        <v>8.8690052447872016</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>9.6219423121418117</v>
+        <v>-6.4257010967688455</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1837357633525158</v>
+        <v>1.6195593212831039</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>4.92988478296812</v>
+        <v>7.1753631514595941</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>5.9997904778384417</v>
+        <v>-0.28575731004203497</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>11.565343167382878</v>
+        <v>0.12870372543924447</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.28701793511395657</v>
+        <v>-0.85143449847063835</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47794711924280087</v>
+        <v>7.6916793919679165</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.9169143239175028E-2</v>
+        <v>-3.8843568885963391</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.974934503935053</v>
+        <v>4.9300028103689453</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>12.868331097283885</v>
+        <v>5.2039052957588741</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7664069135671605</v>
+        <v>1.8416544407831754</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.6428232858618781</v>
+        <v>-6.249481363786356</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.0882773954306337</v>
+        <v>2.3724637707304641</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6748979109996345</v>
+        <v>7.7105745931348508</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>8.968972957507571</v>
+        <v>12.26327018140989</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.3186662016248194</v>
+        <v>1.7781791746524735</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0745562019278569</v>
+        <v>-5.6239665491276334</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7557050230098277</v>
+        <v>9.6353770776507588</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>12.404764897572619</v>
+        <v>-4.5552625937329037</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.5409946513488859</v>
+        <v>-3.9455686933051597</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>12.822877810438587</v>
+        <v>5.5501702168038243</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1495039208669446</v>
+        <v>8.9034464675591032</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2543728644665411</v>
+        <v>-6.894123296173893</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>9.3726219132788628</v>
+        <v>6.2291301575384939</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.3306565690958738</v>
+        <v>-1.5609232606076837</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.4717936160324996</v>
+        <v>-3.8061969513003806</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.4620398190978268</v>
+        <v>11.172603238303548</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7743805119373501</v>
+        <v>-6.2974428119398489</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5358877155764645</v>
+        <v>-9.5976480616697835E-2</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.97894152826293368</v>
+        <v>0.26434057667791233</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4856730717833209</v>
+        <v>-5.9353172533714798</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.0267869651735069</v>
+        <v>-4.2119985571788137</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.3186271436691221</v>
+        <v>12.167104566945842</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7153867306177677</v>
+        <v>12.459429947588205</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.2146635797887599</v>
+        <v>-3.7477224286224446</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15162631981739239</v>
+        <v>3.2511779303658539</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>8.9956284416779067</v>
+        <v>10.38104047829999</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6776166325824722</v>
+        <v>9.209355955981728</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>12.849682742121701</v>
+        <v>-6.3474347175740995</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.9641371833192638</v>
+        <v>11.794526874515856</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>9.8778332341600894</v>
+        <v>-1.1168876567120023</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>9.8705272487511877</v>
+        <v>-1.1246515280760825</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>4.1299327403831114</v>
+        <v>-0.85864724562154926</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>9.5317043072971579</v>
+        <v>-2.7557717678508258</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.7690770826628395</v>
+        <v>12.911725061022992</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.0738671639939437</v>
+        <v>1.19918011696622</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1828099050299254</v>
+        <v>6.6624794892729504</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.0040301910868186</v>
+        <v>12.329392291561302</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4426129599439541</v>
+        <v>3.6753504655568996</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.9021526827979063</v>
+        <v>1.6877248506845994</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.0153887424949675</v>
+        <v>-4.7987267838477141</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>12.248118665101114</v>
+        <v>-6.2573829739002234</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>3.6714456777682933</v>
+        <v>-3.1538177513456316</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8889737433046268</v>
+        <v>-1.6055048265190042</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>10.898293159312605</v>
+        <v>3.0142870027615221</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3542050276745243</v>
+        <v>-1.9553701081872203</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.6030997826038362</v>
+        <v>-5.1477994747923059</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4064064372774965</v>
+        <v>9.5821111091299223</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8867215583704038</v>
+        <v>-1.8836159467611395</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7184284852745577</v>
+        <v>-6.1611912116791894</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.19053731369674765</v>
+        <v>-5.2628276277067165</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.9055557962288816</v>
+        <v>7.9226906002574431</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.26301175065804472</v>
+        <v>10.051074140433474</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>8.0863945063287126</v>
+        <v>1.5410437588277404</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>6.5206929391913953</v>
+        <v>6.9242813841989772</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>10.53926388567783</v>
+        <v>-5.3194076907820165</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4380259842876715</v>
+        <v>8.2653160205195544</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9805383332973179</v>
+        <v>2.7713984171367922</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>10.753991730010735</v>
+        <v>10.548528056425827</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2042574767717618</v>
+        <v>-5.9105294960113568</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>10.980225896807084</v>
+        <v>-2.9563638648006219</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.5937771017389633</v>
+        <v>5.150524061489854</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.4444795480308912</v>
+        <v>0.24371424069915726</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>3.7590677476964522</v>
+        <v>3.133270704384195</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4766044742771491</v>
+        <v>10.926454166341628</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.5038533521265958</v>
+        <v>8.6060181030530138</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.7639567972384071</v>
+        <v>9.9541161470635124</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9813817550235679</v>
+        <v>11.521901848326429</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7611624055916941</v>
+        <v>10.531061797894559</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>6.5885140553478116</v>
+        <v>3.4560467302000539</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.9543452620693937</v>
+        <v>9.0530480187862565</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8799910479537125</v>
+        <v>-0.36362887847410086</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>9.0829804662033453</v>
+        <v>3.2263878125689054</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.55420224026986098</v>
+        <v>4.0627285185572326</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7201694974175528</v>
+        <v>8.9647782515774423</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v>8.3197304392657472</v>
+        <v>-6.9166744597674228</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="1"/>
-        <v>10.812484097793842</v>
+        <v>7.0445206999861263</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.0283627564354472</v>
+        <v>7.5056652418625305</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5608983089544726</v>
+        <v>-4.0098558836400375</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>8.9410081834864172</v>
+        <v>10.289060261307089</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>10.176287673562637</v>
+        <v>10.979867864132938</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>6.6965767941797765</v>
+        <v>12.663525674547088</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9485355571364273</v>
+        <v>-0.91314948770169924</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.3098747623726013</v>
+        <v>8.0711178888926067</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.4845729317117033</v>
+        <v>6.8574500098760023</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3680127790787395</v>
+        <v>7.696819813227485</v>
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.43644802528630056</v>
+        <v>6.5564970925001642</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.585246951729216</v>
+        <v>-0.18918504049770135</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.177635089615785</v>
+        <v>7.5635561306542698</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>10.995111040369004</v>
+        <v>8.8036501343664284</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7516187865809663</v>
+        <v>6.5070400362880445</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.4688730983052292</v>
+        <v>7.2825738859902991</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>10.898531276925979</v>
+        <v>8.493507623798914</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>9.0917384481354091</v>
+        <v>2.4527025304007228</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>5.1297495231482593</v>
+        <v>10.926267529423178</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9937619708791701</v>
+        <v>10.727440109914998</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="1"/>
-        <v>6.115637849993135</v>
+        <v>0.22299358164868721</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>6.7240189157490526</v>
+        <v>-6.4667884845434047</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22186106735592137</v>
+        <v>-5.8623562522476673</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.8194414677192245</v>
+        <v>9.2245135399203662</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6521018720647529</v>
+        <v>9.3988608512515412</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.44556798415304844</v>
+        <v>2.1633672377668489</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8048946094560119</v>
+        <v>11.8081116567359</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.3748443841524196</v>
+        <v>-4.6100890416885081</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>11.943783100608204</v>
+        <v>10.441129701356456</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="1"/>
-        <v>4.438282312636602</v>
+        <v>9.4401250278033899</v>
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="1"/>
-        <v>5.2161493374772796</v>
+        <v>-4.0454374669957449</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38165095223331846</v>
+        <v>-1.0040246825022363</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9673843431562155</v>
+        <v>-1.5578423077539387</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>4.035114587154693</v>
+        <v>-5.7470838341435702</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>8.8702474572496222</v>
+        <v>11.026019417052211</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>7.2558603269017539</v>
+        <v>6.6233142608309983</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6998511041536943</v>
+        <v>-2.6682522074821744</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>10.846724997766856</v>
+        <v>9.1387361754182699</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>11.712770555050508</v>
+        <v>0.37713303342490523</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.9613721531772645</v>
+        <v>1.7324440823545313</v>
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.5446607706577731</v>
+        <v>0.49826378700875207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use 2 arrays for diagonal and off-diagonal elements
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/BiDiagDecompTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/BiDiagDecompTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="300" windowWidth="24915" windowHeight="6465" activeTab="5"/>
+    <workbookView xWindow="4575" yWindow="300" windowWidth="24915" windowHeight="6465"/>
   </bookViews>
   <sheets>
     <sheet name="Upper Thin 10x3" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,15 +86,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,11 +104,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -143,23 +131,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -459,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI77"/>
+  <dimension ref="A1:AI78"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4000,7 +3985,7 @@
         <v>8.8817841970012523E-16</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" ref="A65:A73" si="76">AG52</f>
         <v>7.310494211901453E-16</v>
@@ -4014,7 +3999,7 @@
         <v>0.38196055250832472</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="76"/>
         <v>-1.0094684939496983E-15</v>
@@ -4028,7 +4013,7 @@
         <v>-30.651378914612064</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="76"/>
         <v>-1.8385961586756272E-17</v>
@@ -4042,7 +4027,7 @@
         <v>-5.5511151231257827E-16</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="76"/>
         <v>3.1256835270909162E-18</v>
@@ -4056,7 +4041,7 @@
         <v>3.5527136788005009E-15</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="76"/>
         <v>1.4024283862467174E-15</v>
@@ -4070,7 +4055,7 @@
         <v>4.4408920985006262E-15</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="76"/>
         <v>-4.5251892099652144E-16</v>
@@ -4084,7 +4069,7 @@
         <v>8.8817841970012523E-16</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="76"/>
         <v>2.9163031188788019E-16</v>
@@ -4098,7 +4083,7 @@
         <v>-2.7755575615628914E-17</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="76"/>
         <v>-2.9686478181005755E-16</v>
@@ -4112,7 +4097,7 @@
         <v>2.2204460492503131E-15</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="76"/>
         <v>5.099309236458049E-17</v>
@@ -4126,41 +4111,43 @@
         <v>-3.5527136788005009E-15</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B76">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <f>-F3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f>A64</f>
         <v>-35.202840794458623</v>
       </c>
-      <c r="B77" s="2">
-        <f>F15</f>
-        <v>22.007036325881806</v>
-      </c>
-      <c r="C77" s="1">
-        <f>F28</f>
-        <v>26.302802681853521</v>
-      </c>
-      <c r="D77" s="2">
-        <f>C52</f>
+      <c r="B77">
+        <f>B65</f>
+        <v>26.302802681853514</v>
+      </c>
+      <c r="C77">
+        <f>C66</f>
+        <v>-30.651378914612064</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f>B64</f>
+        <v>22.00703632588181</v>
+      </c>
+      <c r="B78">
+        <f>C65</f>
         <v>0.38196055250832472</v>
       </c>
-      <c r="E77" s="1">
-        <f>-F51</f>
-        <v>-30.651378914612071</v>
-      </c>
-      <c r="F77" s="4">
+      <c r="C78">
         <v>0</v>
       </c>
     </row>
@@ -4171,10 +4158,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W40"/>
+  <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5500,7 +5487,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -5508,7 +5495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="array" ref="A34:E36">MMULT(A27:E29,S26:W30)</f>
         <v>61.754302259114368</v>
@@ -5526,7 +5513,7 @@
         <v>1.12702958474281E-14</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-1.2021353108263053E-14</v>
       </c>
@@ -5543,7 +5530,7 @@
         <v>-6.4168598249874099E-16</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>-9.0927999070751434E-15</v>
       </c>
@@ -5560,41 +5547,43 @@
         <v>-1.7763568394002505E-15</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B39">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
         <f>A34</f>
         <v>61.754302259114368</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40">
+        <f>B35</f>
+        <v>-37.912589241029323</v>
+      </c>
+      <c r="C40">
+        <f>C36</f>
+        <v>-23.51355376739868</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
         <f>B34</f>
         <v>-53.11744231855819</v>
       </c>
-      <c r="C40" s="1">
-        <f>B35</f>
-        <v>-37.912589241029323</v>
-      </c>
-      <c r="D40" s="2">
+      <c r="B41">
         <f>C35</f>
         <v>-19.237585069302259</v>
       </c>
-      <c r="E40" s="1">
-        <f>C36</f>
-        <v>-23.51355376739868</v>
-      </c>
-      <c r="F40" s="2">
+      <c r="C41">
         <f>D36</f>
         <v>19.095330302013426</v>
       </c>
@@ -5606,10 +5595,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V53"/>
+  <dimension ref="A1:V54"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:J13"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7432,7 +7421,7 @@
         <v>4.1219356118994659</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>-4.2001060679924868E-16</v>
       </c>
@@ -7446,49 +7435,51 @@
         <v>11.923337410786642</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B52">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
         <f>A45</f>
         <v>-13.805227697096377</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53">
+        <f>B46</f>
+        <v>-11.766808386262841</v>
+      </c>
+      <c r="C53">
+        <f>C47</f>
+        <v>4.4453729439784722</v>
+      </c>
+      <c r="D53">
+        <f>D48</f>
+        <v>4.1219356118994659</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
         <f>A46</f>
         <v>9.0332337813421262</v>
       </c>
-      <c r="C53" s="1">
-        <f>B46</f>
-        <v>-11.766808386262841</v>
-      </c>
-      <c r="D53" s="2">
+      <c r="B54">
         <f>B47</f>
         <v>7.9579652905572669</v>
       </c>
-      <c r="E53" s="1">
-        <f>C47</f>
-        <v>4.4453729439784722</v>
-      </c>
-      <c r="F53" s="2">
+      <c r="C54">
         <f>C48</f>
         <v>3.4903229856050806</v>
       </c>
-      <c r="G53" s="1">
-        <f>D48</f>
-        <v>4.1219356118994659</v>
-      </c>
-      <c r="H53" s="2">
+      <c r="D54">
         <f>D49</f>
         <v>11.923337410786642</v>
       </c>
@@ -7500,10 +7491,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z66"/>
+  <dimension ref="A1:Z67"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10095,44 +10086,46 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B65">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
         <f>A59</f>
         <v>12.401225109178808</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66">
+        <f>B60</f>
+        <v>-20.725608363515811</v>
+      </c>
+      <c r="C66">
+        <f>C61</f>
+        <v>10.91394389595316</v>
+      </c>
+      <c r="D66">
+        <f>D62</f>
+        <v>9.3999696866547335</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
         <f>A60</f>
         <v>10.060612436440028</v>
       </c>
-      <c r="C66" s="1">
-        <f>B60</f>
-        <v>-20.725608363515811</v>
-      </c>
-      <c r="D66" s="2">
+      <c r="B67">
         <f>B61</f>
         <v>8.3791833460186691</v>
       </c>
-      <c r="E66" s="1">
-        <f>C61</f>
-        <v>10.91394389595316</v>
-      </c>
-      <c r="F66" s="2">
+      <c r="C67">
         <f>C62</f>
         <v>-10.879145778962963</v>
       </c>
-      <c r="G66" s="1">
-        <f>D62</f>
-        <v>9.3999696866547335</v>
-      </c>
-      <c r="H66" s="4">
+      <c r="D67">
         <v>0</v>
       </c>
     </row>
@@ -10143,10 +10136,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W59"/>
+  <dimension ref="A1:W60"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12660,50 +12653,52 @@
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B58">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+      <c r="A59">
         <f>A51</f>
         <v>-16.376621736744926</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59">
+        <f>B52</f>
+        <v>-13.360602120706634</v>
+      </c>
+      <c r="C59">
+        <f>C53</f>
+        <v>12.130118162682122</v>
+      </c>
+      <c r="D59">
+        <f>D54</f>
+        <v>10.853641052475476</v>
+      </c>
+      <c r="E59">
+        <f>E55</f>
+        <v>1.8929822833086383</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A60">
         <f>B51</f>
         <v>19.048293899863783</v>
       </c>
-      <c r="C59" s="1">
-        <f>B52</f>
-        <v>-13.360602120706634</v>
-      </c>
-      <c r="D59" s="2">
+      <c r="B60">
         <f>C52</f>
         <v>-8.8257525120203635</v>
       </c>
-      <c r="E59" s="1">
-        <f>C53</f>
-        <v>12.130118162682122</v>
-      </c>
-      <c r="F59" s="2">
+      <c r="C60">
         <f>D53</f>
         <v>9.6353837408420802</v>
       </c>
-      <c r="G59" s="1">
-        <f>D54</f>
-        <v>10.853641052475476</v>
-      </c>
-      <c r="H59" s="2">
+      <c r="D60">
         <f>E54</f>
         <v>5.3976823138998444</v>
       </c>
-      <c r="I59" s="1">
-        <f>E55</f>
-        <v>1.8929822833086383</v>
-      </c>
-      <c r="J59" s="4">
+      <c r="E60">
         <v>0</v>
       </c>
     </row>
@@ -12714,10 +12709,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W67"/>
+  <dimension ref="A1:W68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="J67" sqref="J67"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15343,57 +15338,60 @@
         <v>3.9430916136518879</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B66">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
         <f>A59</f>
         <v>13.22383041048691</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67">
+        <f>B60</f>
+        <v>10.029480829982248</v>
+      </c>
+      <c r="C67">
+        <f>C61</f>
+        <v>-9.375552303994434</v>
+      </c>
+      <c r="D67">
+        <f>D62</f>
+        <v>-12.636859495657063</v>
+      </c>
+      <c r="E67">
+        <f>E63</f>
+        <v>3.9430916136518879</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
         <f>A60</f>
         <v>-10.428889816627075</v>
       </c>
-      <c r="C67" s="1">
-        <f>B60</f>
-        <v>10.029480829982248</v>
-      </c>
-      <c r="D67" s="2">
+      <c r="B68">
         <f>B61</f>
         <v>12.689373764613437</v>
       </c>
-      <c r="E67" s="1">
-        <f>C61</f>
-        <v>-9.375552303994434</v>
-      </c>
-      <c r="F67" s="2">
+      <c r="C68">
         <f>C62</f>
         <v>10.804400419442402</v>
       </c>
-      <c r="G67" s="1">
-        <f>D62</f>
-        <v>-12.636859495657063</v>
-      </c>
-      <c r="H67" s="2">
+      <c r="D68">
         <f>D63</f>
         <v>8.9499466373636114</v>
       </c>
-      <c r="I67" s="1">
-        <f>E63</f>
-        <v>3.9430916136518879</v>
-      </c>
-      <c r="J67" s="4">
+      <c r="E68">
+        <f>E64</f>
         <v>0</v>
       </c>
     </row>
@@ -15415,1051 +15413,1051 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*20-7</f>
-        <v>12.041620907257133</v>
+        <v>1.8780692928904621</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:J16" ca="1" si="0">RAND()*20-7</f>
-        <v>-4.5802676133425244</v>
+        <v>-1.9058069086160323</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>9.3088409042958382</v>
+        <v>-6.2188866695836502</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.6930478936307818</v>
+        <v>-2.2803922897043982</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.3750324880874221</v>
+        <v>11.613069819194834</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>10.671306160962942</v>
+        <v>3.3675202766236811</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0068654950857159</v>
+        <v>-0.99814416497920266</v>
       </c>
       <c r="H1">
         <f t="shared" ca="1" si="0"/>
-        <v>11.31171318170583</v>
+        <v>5.3880744203235054</v>
       </c>
       <c r="I1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1899712577687911</v>
+        <v>-0.45041827363667508</v>
       </c>
       <c r="J1">
         <f t="shared" ca="1" si="0"/>
-        <v>11.982372606055606</v>
+        <v>2.2084165390049026</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:J25" ca="1" si="1">RAND()*20-7</f>
-        <v>11.040020259804567</v>
+        <v>9.7996075072550646</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>8.650627484989176</v>
+        <v>8.5914756242466126</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7058279279778219</v>
+        <v>0.48068588668702006</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0627199231574824</v>
+        <v>7.0599160726910917</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>10.75817091785807</v>
+        <v>-2.714550522028401</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2669898275966371</v>
+        <v>-5.4468301767554088</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.1117722051896237</v>
+        <v>2.7410453230477678</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1052114381397722</v>
+        <v>-6.4590313963554244</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.30174037270263021</v>
+        <v>4.4728915034825292</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5855014627110684</v>
+        <v>0.62339495318516747</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.82951939429402799</v>
+        <v>6.0778424513025708</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2017333660497442E-2</v>
+        <v>-5.8702114602693101</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.7766554027024783</v>
+        <v>-2.3040292956728656</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2559003668537994</v>
+        <v>8.365216710975691</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3024008114219168</v>
+        <v>5.1385140535090557</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>12.295908047108579</v>
+        <v>10.880465134628441</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.0198049862516783E-2</v>
+        <v>3.6976922623041233</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.4421318893783939</v>
+        <v>5.2417617318435106</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4332526004210786</v>
+        <v>6.3260608433856813</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.56263882823073</v>
+        <v>7.6484182003180141</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>12.702803793125113</v>
+        <v>-4.8981339129496897</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>12.186786362075701</v>
+        <v>-3.5741513861239675</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.3103405842571791</v>
+        <v>9.3008528362522256</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6783787927134775</v>
+        <v>-1.1406838121570866</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3301887354713813</v>
+        <v>-1.4265961772156643</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.6150199462329318</v>
+        <v>-2.0615274664329419</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7557936953498157</v>
+        <v>-4.614650861946517</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4454147112899722</v>
+        <v>9.1461305487942077</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.134031697531154</v>
+        <v>8.1608865899992278</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>11.898068851429066</v>
+        <v>-3.3382250654539152</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.2737377261350877</v>
+        <v>5.9680350731492382</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6898886414609926</v>
+        <v>3.0753035876077224</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>8.3548418855072288</v>
+        <v>5.7111993060724942</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.8025507530212632</v>
+        <v>-0.67720756039431773</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.7222318668603553</v>
+        <v>6.2575373936806216</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.5873423305145433</v>
+        <v>2.4564304458419954</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.3159895327820053E-3</v>
+        <v>-5.9597714751882069</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0348438693420157</v>
+        <v>0.96044909366132991</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.80268828152004</v>
+        <v>8.7143253236285396</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>2.189298359896279</v>
+        <v>10.755856717018055</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>12.977699517501598</v>
+        <v>-2.5291928637884897</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1611918759469742</v>
+        <v>9.0630177469316209</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.7413077471102447</v>
+        <v>9.4864365790965586</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2366711097496683</v>
+        <v>6.8668464171635542</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9153586148973858</v>
+        <v>3.5827908811892222</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>8.7894594954153114</v>
+        <v>0.93847429988699105</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.1436967593069056</v>
+        <v>-3.5100484840260697</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8162087810901095</v>
+        <v>5.5292250836681074</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>10.816626076116126</v>
+        <v>-3.963138657864183</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>9.4373103146605182</v>
+        <v>9.9740490290213479</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7252795755223858</v>
+        <v>-3.5856424757187959</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>11.819411554080578</v>
+        <v>6.4537761641286231</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5421868592796457</v>
+        <v>-5.0682350658842505</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>8.7068351092706138</v>
+        <v>10.685171952612645</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1229266747658713</v>
+        <v>0.31254754146541064</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>9.9123475772176164</v>
+        <v>10.763139689135773</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7833414032390351</v>
+        <v>-0.77026541246210556</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>7.8882287307315568</v>
+        <v>-2.6002032304126743</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6304564941224751</v>
+        <v>-0.54216226150573021</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.0652368150552172</v>
+        <v>-2.4797901676397913</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.16510134525659126</v>
+        <v>3.9156410940575928</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1698609455114859</v>
+        <v>1.6085224772901761</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.55286468444132808</v>
+        <v>-1.3005494948420253</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>12.587830323206255</v>
+        <v>8.7467611715913591</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4333108635557128</v>
+        <v>6.1236029511346892</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>9.591726815871418</v>
+        <v>12.54322864120768</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.7198612288885173</v>
+        <v>-6.7941381608970302</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5133560404554736</v>
+        <v>8.0055512081221565</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>9.407777887627077</v>
+        <v>7.8716160845764662</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>11.81449860195746</v>
+        <v>-4.3059886994656953</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>11.658673447065215</v>
+        <v>4.4448891392274721</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.7895845498578771</v>
+        <v>0.74789664533392486</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2917591983076147</v>
+        <v>11.844905025808924</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3762746644241588</v>
+        <v>-4.184122875343979</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7399402716869794</v>
+        <v>1.4761218373036566</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2914455972573933</v>
+        <v>-4.6403871745149443</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.7087814931833689</v>
+        <v>0.5374361067260498</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8231965596670676</v>
+        <v>10.227693912012793</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5394391625247472</v>
+        <v>6.5329029778850263</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4186912033654764</v>
+        <v>8.9589626570164249</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.2363366003471956</v>
+        <v>7.3617021037544319</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>11.167014452695437</v>
+        <v>9.5038387906916775</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>11.335236052215677</v>
+        <v>5.5324804785841852</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>9.468548460740724</v>
+        <v>8.2731495769165981</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2731258442186739</v>
+        <v>10.504452270553855</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0590523907088745</v>
+        <v>10.202838522232391</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.0659589986443709</v>
+        <v>0.442865242705059</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.0459255803909748</v>
+        <v>-1.8148939396821744</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9440622972496904</v>
+        <v>8.38820825170896</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>12.401851484455982</v>
+        <v>-1.7280476493309216</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6906785032984999</v>
+        <v>7.4091362750752268</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3507642644073963</v>
+        <v>-2.4647102673804788</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.6558523203923121</v>
+        <v>8.1076738614918469</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4522642723228341</v>
+        <v>7.1638012315945865</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0640116177586059</v>
+        <v>-3.8047590056584673</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5547108789325499</v>
+        <v>2.1429239072034569</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>9.4990791901873166</v>
+        <v>4.0435691982695889</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.3416867617683153E-2</v>
+        <v>-1.0903217593234364</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11098712149333068</v>
+        <v>2.8109840667071584</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>11.626530142484462</v>
+        <v>11.398007342914081</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>6.8579620280517339</v>
+        <v>-6.0028640209543509</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1298604161687038</v>
+        <v>6.5934448140676327</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1021371692975315</v>
+        <v>10.345169528491571</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9935676514544944</v>
+        <v>4.7781636928478406</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2743617182991009</v>
+        <v>3.4318496787740234</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5837313671474558</v>
+        <v>-0.792108587912983</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.6936179671346459</v>
+        <v>10.737454145958885</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7352442388976446</v>
+        <v>-3.2705260341944924</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>11.321012189351379</v>
+        <v>3.8191626976535016</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2548770238295592</v>
+        <v>-0.34162717681497412</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.9701736316058049</v>
+        <v>2.2976630572908903</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>11.666111087384781</v>
+        <v>11.192128784911258</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>8.8690052447872016</v>
+        <v>2.4317223814549891</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.4257010967688455</v>
+        <v>0.81384571022963659</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6195593212831039</v>
+        <v>0.44512432232282961</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>7.1753631514595941</v>
+        <v>6.1846489441018697</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.28575731004203497</v>
+        <v>12.110781044834305</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12870372543924447</v>
+        <v>8.2034214873016609</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.85143449847063835</v>
+        <v>8.3047660056528194</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>7.6916793919679165</v>
+        <v>6.8003270734540102</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.8843568885963391</v>
+        <v>-1.7609984373177099</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9300028103689453</v>
+        <v>-2.2617854009079013</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2039052957588741</v>
+        <v>3.4910157862036346</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8416544407831754</v>
+        <v>6.0385149594435195</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.249481363786356</v>
+        <v>-5.9051904747500243</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3724637707304641</v>
+        <v>-3.4983631403681197</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7105745931348508</v>
+        <v>-2.339176101768965</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>12.26327018140989</v>
+        <v>6.0265704160965097</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7781791746524735</v>
+        <v>4.0218612879254589</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.6239665491276334</v>
+        <v>6.5824008998934058</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>9.6353770776507588</v>
+        <v>8.7748209902040522</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.5552625937329037</v>
+        <v>7.4218165115802925</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.9455686933051597</v>
+        <v>-1.2356628613482279</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5501702168038243</v>
+        <v>10.190606762986658</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>8.9034464675591032</v>
+        <v>0.11837748113429214</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.894123296173893</v>
+        <v>1.5110361148724252</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2291301575384939</v>
+        <v>-2.0634813851023548</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.5609232606076837</v>
+        <v>2.9028626535807298</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.8061969513003806</v>
+        <v>-1.3363403545958956</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>11.172603238303548</v>
+        <v>-5.1876963668759295</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.2974428119398489</v>
+        <v>6.1580818018783887</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.5976480616697835E-2</v>
+        <v>-5.1648782185380675</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26434057667791233</v>
+        <v>-1.3925068781968113</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.9353172533714798</v>
+        <v>-6.3643151430267224</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.2119985571788137</v>
+        <v>10.261866040873397</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>12.167104566945842</v>
+        <v>-5.6306053506874676E-2</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>12.459429947588205</v>
+        <v>-6.9040592890805579</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.7477224286224446</v>
+        <v>-1.0460078528750953</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2511779303658539</v>
+        <v>2.0639388848468307</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>10.38104047829999</v>
+        <v>-5.4821487069642032</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>9.209355955981728</v>
+        <v>-1.8832293658506671</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.3474347175740995</v>
+        <v>12.345766568787635</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>11.794526874515856</v>
+        <v>4.1088866557001342</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.1168876567120023</v>
+        <v>-1.6389228373733982</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.1246515280760825</v>
+        <v>3.0440705130370986</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.85864724562154926</v>
+        <v>10.630759137005317</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.7557717678508258</v>
+        <v>-0.3453115927191952</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>12.911725061022992</v>
+        <v>1.5805832787509573</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.19918011696622</v>
+        <v>9.51572107269158</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>6.6624794892729504</v>
+        <v>12.576766925567004</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>12.329392291561302</v>
+        <v>1.2608484890326963</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>3.6753504655568996</v>
+        <v>-5.4439774774617167</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6877248506845994</v>
+        <v>7.1065394585364068</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.7987267838477141</v>
+        <v>4.6302366929252337</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.2573829739002234</v>
+        <v>1.5196643563234904</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.1538177513456316</v>
+        <v>4.8702170331971999</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.6055048265190042</v>
+        <v>6.2867633679342241</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0142870027615221</v>
+        <v>11.870524758262704</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.9553701081872203</v>
+        <v>-4.3326514373409646</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.1477994747923059</v>
+        <v>-1.2634605915903663</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>9.5821111091299223</v>
+        <v>2.1831632845559685</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.8836159467611395</v>
+        <v>4.3827111034164545</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.1611912116791894</v>
+        <v>-1.2031547159279654</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.2628276277067165</v>
+        <v>-2.9447523932829105</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>7.9226906002574431</v>
+        <v>8.5075370595021838</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>10.051074140433474</v>
+        <v>-4.8155133638118679</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5410437588277404</v>
+        <v>2.6210572376338419</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>6.9242813841989772</v>
+        <v>0.11849205953772657</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.3194076907820165</v>
+        <v>-1.9509940550203213</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>8.2653160205195544</v>
+        <v>-5.3029616806446382</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7713984171367922</v>
+        <v>9.1725978147357381</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>10.548528056425827</v>
+        <v>-4.7447029869579325</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.9105294960113568</v>
+        <v>12.347878851677081</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.9563638648006219</v>
+        <v>10.397799067781552</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>5.150524061489854</v>
+        <v>2.7827637098650371</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24371424069915726</v>
+        <v>1.7133435352256967</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>3.133270704384195</v>
+        <v>5.4228383378022329</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>10.926454166341628</v>
+        <v>7.5353026347143395</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6060181030530138</v>
+        <v>11.393351542099829</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="1"/>
-        <v>9.9541161470635124</v>
+        <v>6.1621633983746307</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>11.521901848326429</v>
+        <v>-3.0977994493840715</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>10.531061797894559</v>
+        <v>-0.51900489776743441</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4560467302000539</v>
+        <v>3.689684280252127</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>9.0530480187862565</v>
+        <v>2.6136452155431673</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.36362887847410086</v>
+        <v>10.789109837526119</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2263878125689054</v>
+        <v>1.8149401200183934</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>4.0627285185572326</v>
+        <v>-0.14315281415519188</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>8.9647782515774423</v>
+        <v>11.09918417500279</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.9166744597674228</v>
+        <v>3.2819243153036499</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0445206999861263</v>
+        <v>7.6191150445290212</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>7.5056652418625305</v>
+        <v>-2.5349216019938252</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.0098558836400375</v>
+        <v>11.445896831955196</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>10.289060261307089</v>
+        <v>7.4997903336462102</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>10.979867864132938</v>
+        <v>2.4082580253142485</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>12.663525674547088</v>
+        <v>-0.41884604815502868</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.91314948770169924</v>
+        <v>11.252338036399735</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>8.0711178888926067</v>
+        <v>12.467704783039995</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>6.8574500098760023</v>
+        <v>7.7235268762723042</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
-        <v>7.696819813227485</v>
+        <v>-4.9154099510928528</v>
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="1"/>
-        <v>6.5564970925001642</v>
+        <v>3.5950441658136256</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.18918504049770135</v>
+        <v>0.98550891899704141</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>7.5635561306542698</v>
+        <v>-3.0267263247703928</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>8.8036501343664284</v>
+        <v>4.4802049701870441</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>6.5070400362880445</v>
+        <v>-0.91856676694799066</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>7.2825738859902991</v>
+        <v>0.23090609116438632</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>8.493507623798914</v>
+        <v>2.8378016347438866</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4527025304007228</v>
+        <v>-0.74412529792708781</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>10.926267529423178</v>
+        <v>3.4525547497903037</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="1"/>
-        <v>10.727440109914998</v>
+        <v>10.894016550736755</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22299358164868721</v>
+        <v>2.4924663815548769</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.4667884845434047</v>
+        <v>12.400222963535324</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.8623562522476673</v>
+        <v>-3.1971194873116442</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>9.2245135399203662</v>
+        <v>0.47506366281157408</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3988608512515412</v>
+        <v>8.7222968304401469</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1633672377668489</v>
+        <v>-0.75027102813005264</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>11.8081116567359</v>
+        <v>7.2700258790011389</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.6100890416885081</v>
+        <v>9.9263599884104821</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>10.441129701356456</v>
+        <v>-1.4014112474414961</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="1"/>
-        <v>9.4401250278033899</v>
+        <v>12.449786104964158</v>
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.0454374669957449</v>
+        <v>0.98653688869161993</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.0040246825022363</v>
+        <v>1.7136741213777196</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.5578423077539387</v>
+        <v>8.8386948159781031</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.7470838341435702</v>
+        <v>12.74245640302162</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>11.026019417052211</v>
+        <v>-2.2599440424824788</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>6.6233142608309983</v>
+        <v>3.2670458547374679</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.6682522074821744</v>
+        <v>0.24150575584721246</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1387361754182699</v>
+        <v>12.448453784124176</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.37713303342490523</v>
+        <v>3.0758343017064433</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7324440823545313</v>
+        <v>2.6714159990320177</v>
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49826378700875207</v>
+        <v>-4.877351284649885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>